<commit_message>
V4.0 | 11.30.2025 -CICD- 11/29/2025 7:17:01 PM
</commit_message>
<xml_diff>
--- a/Carga Masiva/CargaMaterialesAcrux.xlsx
+++ b/Carga Masiva/CargaMaterialesAcrux.xlsx
@@ -1,26 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepositoriosAEC\Acrux-Release\Carga Masiva\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RepositoriosAEC\Acrux-Release\Carga Masiva\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB4C9A4-BA92-4AA4-ACAE-15E9A09F3DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C085532E-5E05-4D96-B75C-1A2C205F10FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CargaMaterialesAcrux" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>TIPO INVENTARIO</t>
   </si>
@@ -167,6 +181,12 @@
   </si>
   <si>
     <t>0-0-0</t>
+  </si>
+  <si>
+    <t>CODIGO REFERENCIA2</t>
+  </si>
+  <si>
+    <t>REF2</t>
   </si>
 </sst>
 </file>
@@ -1016,36 +1036,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2:AD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="26" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="27" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1059,85 +1080,88 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1151,81 +1175,84 @@
         <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>500</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>1000</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>500</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <v>100</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>50</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>150</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>1</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>33</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>34</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>35</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>36</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>37</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>38</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>40</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>41</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>42</v>
-      </c>
-      <c r="AB2">
-        <v>1</v>
       </c>
       <c r="AC2">
         <v>1</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>